<commit_message>
Fixed Delete Bill, Added e_id and w_id
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -59,70 +59,100 @@
     <t>2</t>
   </si>
   <si>
-    <t>1ST FLOOR</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Tester</t>
+    <t>ALL SECTIONS</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A's</t>
+  </si>
+  <si>
+    <t>B's</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>CHICKEN</t>
+  </si>
+  <si>
+    <t>C's</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>2016-10-17</t>
+  </si>
+  <si>
+    <t>RATE/ what to put?</t>
+  </si>
+  <si>
+    <t>LOL AMOUNT</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>ALL SECTIONS</t>
-  </si>
-  <si>
-    <t>12312</t>
-  </si>
-  <si>
-    <t>321</t>
-  </si>
-  <si>
-    <t>2016-10-17</t>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>1332</t>
   </si>
   <si>
     <t>123</t>
   </si>
   <si>
-    <t>RATE/ what to put?</t>
-  </si>
-  <si>
-    <t>LOL AMOUNT</t>
-  </si>
-  <si>
-    <t>4645</t>
-  </si>
-  <si>
-    <t>234</t>
-  </si>
-  <si>
-    <t>1233</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>565</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>FOOD</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>qee</t>
-  </si>
-  <si>
-    <t>314</t>
-  </si>
-  <si>
-    <t>677</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -206,27 +236,27 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -264,262 +294,302 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="F14" t="s">
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
         <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -557,102 +627,142 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
         <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to sections combobox
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -167,6 +167,27 @@
   </si>
   <si>
     <t>1703.72</t>
+  </si>
+  <si>
+    <t>1ST FLOOR</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>FOOD</t>
+  </si>
+  <si>
+    <t>qw</t>
+  </si>
+  <si>
+    <t>qwe</t>
+  </si>
+  <si>
+    <t>nad</t>
   </si>
 </sst>
 </file>
@@ -245,6 +266,76 @@
         <v>17</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added functionality to Search Bar
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -188,6 +188,84 @@
   </si>
   <si>
     <t>nad</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>2ND FLOOR</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>CHICKEN</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>VEGETABLE</t>
+  </si>
+  <si>
+    <t>wew</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>FRUIT</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>GROCERY</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>wer</t>
+  </si>
+  <si>
+    <t>272.00</t>
+  </si>
+  <si>
+    <t>32.00</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>280.00</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>SPECIAL</t>
+  </si>
+  <si>
+    <t>Spec</t>
+  </si>
+  <si>
+    <t>sp</t>
   </si>
 </sst>
 </file>
@@ -336,6 +414,160 @@
         <v>57</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -609,6 +841,66 @@
         <v>43</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>